<commit_message>
Corrected density math to properly account for molar mass - values were otherwise way higher than they should have been!
</commit_message>
<xml_diff>
--- a/CVW5_Atmosphere/Test Data Viewer.xlsx
+++ b/CVW5_Atmosphere/Test Data Viewer.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\CVW5_Atmosphere\CVW5_Atmosphere\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\projects\CVW5_Atmosphere\CVW5_Atmosphere\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28D87F0B-36CF-4D44-9AAB-E2B14BA83970}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F4204F0-9D9C-4F4C-AA60-68A8EEC13D62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15990" xr2:uid="{419E100D-6CEE-4CDA-9761-1BB0795B6021}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="15750" xr2:uid="{419E100D-6CEE-4CDA-9761-1BB0795B6021}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,9 +19,9 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{841E416B-1EF1-43b6-AB56-02D37102CBD5}">
       <x15:pivotCaches>
-        <pivotCache cacheId="45" r:id="rId2"/>
-        <pivotCache cacheId="54" r:id="rId3"/>
-        <pivotCache cacheId="65" r:id="rId4"/>
+        <pivotCache cacheId="5" r:id="rId2"/>
+        <pivotCache cacheId="8" r:id="rId3"/>
+        <pivotCache cacheId="11" r:id="rId4"/>
       </x15:pivotCaches>
     </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{983426D0-5260-488c-9760-48F4B6AC55F4}">
@@ -51,7 +51,7 @@
     <extLst>
       <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{DE250136-89BD-433C-8126-D09CA5730AF9}">
         <x15:connection id="testoutput">
-          <x15:textPr codePage="437" sourceFile="D:\projects\CVW5_Atmosphere\CVW5_AtmoTests\bin\Debug\net48\testoutput.csv" tab="0" comma="1">
+          <x15:textPr codePage="437" sourceFile="K:\projects\CVW5_Atmosphere\CVW5_AtmoTests\bin\Debug\net48\testoutput.csv" tab="0" comma="1">
             <textFields count="4">
               <textField/>
               <textField/>
@@ -279,7 +279,7 @@
           </c:marker>
           <c:cat>
             <c:strLit>
-              <c:ptCount val="62"/>
+              <c:ptCount val="60"/>
               <c:pt idx="0">
                 <c:v>0</c:v>
               </c:pt>
@@ -459,19 +459,13 @@
               </c:pt>
               <c:pt idx="59">
                 <c:v>59000</c:v>
-              </c:pt>
-              <c:pt idx="60">
-                <c:v>60000</c:v>
-              </c:pt>
-              <c:pt idx="61">
-                <c:v>61000</c:v>
               </c:pt>
             </c:strLit>
           </c:cat>
           <c:val>
             <c:numLit>
               <c:formatCode>General</c:formatCode>
-              <c:ptCount val="62"/>
+              <c:ptCount val="60"/>
               <c:pt idx="0">
                 <c:v>288.14999999999998</c:v>
               </c:pt>
@@ -651,12 +645,6 @@
               </c:pt>
               <c:pt idx="59">
                 <c:v>248.25</c:v>
-              </c:pt>
-              <c:pt idx="60">
-                <c:v>245.45</c:v>
-              </c:pt>
-              <c:pt idx="61">
-                <c:v>242.65</c:v>
               </c:pt>
             </c:numLit>
           </c:val>
@@ -968,6 +956,9 @@
       <c:pivotFmt>
         <c:idx val="0"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -1080,6 +1071,9 @@
       <c:pivotFmt>
         <c:idx val="2"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -1107,6 +1101,9 @@
       <c:pivotFmt>
         <c:idx val="3"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -1134,6 +1131,9 @@
       <c:pivotFmt>
         <c:idx val="4"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -1161,6 +1161,9 @@
       <c:pivotFmt>
         <c:idx val="5"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -1188,6 +1191,9 @@
       <c:pivotFmt>
         <c:idx val="6"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -1215,6 +1221,9 @@
       <c:pivotFmt>
         <c:idx val="7"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -1242,6 +1251,9 @@
       <c:pivotFmt>
         <c:idx val="8"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -1269,6 +1281,9 @@
       <c:pivotFmt>
         <c:idx val="9"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -1296,6 +1311,9 @@
       <c:pivotFmt>
         <c:idx val="10"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -1323,6 +1341,9 @@
       <c:pivotFmt>
         <c:idx val="11"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -1350,6 +1371,9 @@
       <c:pivotFmt>
         <c:idx val="12"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -1377,6 +1401,9 @@
       <c:pivotFmt>
         <c:idx val="13"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -1404,6 +1431,9 @@
       <c:pivotFmt>
         <c:idx val="14"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -1431,6 +1461,9 @@
       <c:pivotFmt>
         <c:idx val="15"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -1458,6 +1491,9 @@
       <c:pivotFmt>
         <c:idx val="16"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -1485,6 +1521,9 @@
       <c:pivotFmt>
         <c:idx val="17"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -1512,6 +1551,9 @@
       <c:pivotFmt>
         <c:idx val="18"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -1539,6 +1581,9 @@
       <c:pivotFmt>
         <c:idx val="19"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -1566,6 +1611,9 @@
       <c:pivotFmt>
         <c:idx val="20"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -1593,6 +1641,9 @@
       <c:pivotFmt>
         <c:idx val="21"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -1620,6 +1671,9 @@
       <c:pivotFmt>
         <c:idx val="22"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -1647,6 +1701,9 @@
       <c:pivotFmt>
         <c:idx val="23"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -1674,6 +1731,9 @@
       <c:pivotFmt>
         <c:idx val="24"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -1701,6 +1761,9 @@
       <c:pivotFmt>
         <c:idx val="25"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -1728,6 +1791,9 @@
       <c:pivotFmt>
         <c:idx val="26"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -1755,6 +1821,9 @@
       <c:pivotFmt>
         <c:idx val="27"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -1782,6 +1851,9 @@
       <c:pivotFmt>
         <c:idx val="28"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -1809,6 +1881,9 @@
       <c:pivotFmt>
         <c:idx val="29"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -1836,6 +1911,9 @@
       <c:pivotFmt>
         <c:idx val="30"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -1863,6 +1941,9 @@
       <c:pivotFmt>
         <c:idx val="31"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -1890,6 +1971,9 @@
       <c:pivotFmt>
         <c:idx val="32"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -1917,6 +2001,9 @@
       <c:pivotFmt>
         <c:idx val="33"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -1944,6 +2031,9 @@
       <c:pivotFmt>
         <c:idx val="34"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -1971,6 +2061,9 @@
       <c:pivotFmt>
         <c:idx val="35"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -1998,6 +2091,9 @@
       <c:pivotFmt>
         <c:idx val="36"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -2025,6 +2121,9 @@
       <c:pivotFmt>
         <c:idx val="37"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -2052,6 +2151,9 @@
       <c:pivotFmt>
         <c:idx val="38"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -2079,6 +2181,9 @@
       <c:pivotFmt>
         <c:idx val="39"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -2106,6 +2211,9 @@
       <c:pivotFmt>
         <c:idx val="40"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -2133,6 +2241,9 @@
       <c:pivotFmt>
         <c:idx val="41"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -2160,6 +2271,9 @@
       <c:pivotFmt>
         <c:idx val="42"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -2187,6 +2301,9 @@
       <c:pivotFmt>
         <c:idx val="43"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -2214,6 +2331,9 @@
       <c:pivotFmt>
         <c:idx val="44"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -2241,6 +2361,9 @@
       <c:pivotFmt>
         <c:idx val="45"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -2268,6 +2391,9 @@
       <c:pivotFmt>
         <c:idx val="46"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -2295,6 +2421,9 @@
       <c:pivotFmt>
         <c:idx val="47"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -2322,6 +2451,9 @@
       <c:pivotFmt>
         <c:idx val="48"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -2349,6 +2481,9 @@
       <c:pivotFmt>
         <c:idx val="49"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -2376,6 +2511,9 @@
       <c:pivotFmt>
         <c:idx val="50"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -2403,6 +2541,9 @@
       <c:pivotFmt>
         <c:idx val="51"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -2430,6 +2571,9 @@
       <c:pivotFmt>
         <c:idx val="52"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -2457,6 +2601,9 @@
       <c:pivotFmt>
         <c:idx val="53"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -2484,6 +2631,9 @@
       <c:pivotFmt>
         <c:idx val="54"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -2511,6 +2661,9 @@
       <c:pivotFmt>
         <c:idx val="55"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -2538,6 +2691,9 @@
       <c:pivotFmt>
         <c:idx val="56"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -2565,6 +2721,9 @@
       <c:pivotFmt>
         <c:idx val="57"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -2592,6 +2751,9 @@
       <c:pivotFmt>
         <c:idx val="58"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -2619,6 +2781,9 @@
       <c:pivotFmt>
         <c:idx val="59"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -2646,6 +2811,9 @@
       <c:pivotFmt>
         <c:idx val="60"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -2673,6 +2841,9 @@
       <c:pivotFmt>
         <c:idx val="61"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -2700,6 +2871,9 @@
       <c:pivotFmt>
         <c:idx val="62"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -2727,6 +2901,9 @@
       <c:pivotFmt>
         <c:idx val="63"/>
         <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
           <a:ln w="28575" cap="rnd">
             <a:solidFill>
               <a:schemeClr val="accent1"/>
@@ -2862,7 +3039,7 @@
           </c:marker>
           <c:cat>
             <c:strLit>
-              <c:ptCount val="62"/>
+              <c:ptCount val="60"/>
               <c:pt idx="0">
                 <c:v>0</c:v>
               </c:pt>
@@ -3042,19 +3219,13 @@
               </c:pt>
               <c:pt idx="59">
                 <c:v>59000</c:v>
-              </c:pt>
-              <c:pt idx="60">
-                <c:v>60000</c:v>
-              </c:pt>
-              <c:pt idx="61">
-                <c:v>61000</c:v>
               </c:pt>
             </c:strLit>
           </c:cat>
           <c:val>
             <c:numLit>
               <c:formatCode>General</c:formatCode>
-              <c:ptCount val="62"/>
+              <c:ptCount val="60"/>
               <c:pt idx="0">
                 <c:v>101325</c:v>
               </c:pt>
@@ -3234,12 +3405,6 @@
               </c:pt>
               <c:pt idx="59">
                 <c:v>23.33</c:v>
-              </c:pt>
-              <c:pt idx="60">
-                <c:v>20.31467</c:v>
-              </c:pt>
-              <c:pt idx="61">
-                <c:v>17.661020000000001</c:v>
               </c:pt>
             </c:numLit>
           </c:val>
@@ -3630,7 +3795,7 @@
           </c:marker>
           <c:cat>
             <c:strLit>
-              <c:ptCount val="62"/>
+              <c:ptCount val="60"/>
               <c:pt idx="0">
                 <c:v>0</c:v>
               </c:pt>
@@ -3810,204 +3975,192 @@
               </c:pt>
               <c:pt idx="59">
                 <c:v>59000</c:v>
-              </c:pt>
-              <c:pt idx="60">
-                <c:v>60000</c:v>
-              </c:pt>
-              <c:pt idx="61">
-                <c:v>61000</c:v>
               </c:pt>
             </c:strLit>
           </c:cat>
           <c:val>
             <c:numLit>
               <c:formatCode>General</c:formatCode>
-              <c:ptCount val="62"/>
+              <c:ptCount val="60"/>
               <c:pt idx="0">
-                <c:v>42.292560000000002</c:v>
+                <c:v>1.224979</c:v>
               </c:pt>
               <c:pt idx="1">
-                <c:v>38.37903</c:v>
+                <c:v>1.111626</c:v>
               </c:pt>
               <c:pt idx="2">
-                <c:v>34.748750000000001</c:v>
+                <c:v>1.0064770000000001</c:v>
               </c:pt>
               <c:pt idx="3">
-                <c:v>31.38721</c:v>
+                <c:v>0.90911189999999997</c:v>
               </c:pt>
               <c:pt idx="4">
-                <c:v>28.28031</c:v>
+                <c:v>0.81912209999999996</c:v>
               </c:pt>
               <c:pt idx="5">
-                <c:v>25.41433</c:v>
+                <c:v>0.73611070000000001</c:v>
               </c:pt>
               <c:pt idx="6">
-                <c:v>22.776029999999999</c:v>
+                <c:v>0.65969409999999995</c:v>
               </c:pt>
               <c:pt idx="7">
-                <c:v>20.35257</c:v>
+                <c:v>0.58949980000000002</c:v>
               </c:pt>
               <c:pt idx="8">
-                <c:v>18.13148</c:v>
+                <c:v>0.52516750000000001</c:v>
               </c:pt>
               <c:pt idx="9">
-                <c:v>16.10078</c:v>
+                <c:v>0.46634940000000003</c:v>
               </c:pt>
               <c:pt idx="10">
-                <c:v>14.24883</c:v>
+                <c:v>0.41270869999999998</c:v>
               </c:pt>
               <c:pt idx="11">
-                <c:v>12.564120000000001</c:v>
+                <c:v>0.36391230000000002</c:v>
               </c:pt>
               <c:pt idx="12">
-                <c:v>10.73124</c:v>
+                <c:v>0.31082399999999999</c:v>
               </c:pt>
               <c:pt idx="13">
-                <c:v>9.1657510000000002</c:v>
+                <c:v>0.26548050000000001</c:v>
               </c:pt>
               <c:pt idx="14">
-                <c:v>7.828633</c:v>
+                <c:v>0.2267517</c:v>
               </c:pt>
               <c:pt idx="15">
-                <c:v>6.6865769999999998</c:v>
+                <c:v>0.1936727</c:v>
               </c:pt>
               <c:pt idx="16">
-                <c:v>5.7111270000000003</c:v>
+                <c:v>0.16541939999999999</c:v>
               </c:pt>
               <c:pt idx="17">
-                <c:v>4.8779779999999997</c:v>
+                <c:v>0.14128769999999999</c:v>
               </c:pt>
               <c:pt idx="18">
-                <c:v>4.1663680000000003</c:v>
+                <c:v>0.1206764</c:v>
               </c:pt>
               <c:pt idx="19">
-                <c:v>3.5585710000000002</c:v>
+                <c:v>0.10307189999999999</c:v>
               </c:pt>
               <c:pt idx="20">
-                <c:v>3.039364</c:v>
+                <c:v>8.8033349999999996E-2</c:v>
               </c:pt>
               <c:pt idx="21">
-                <c:v>2.5849820000000001</c:v>
+                <c:v>7.4872469999999997E-2</c:v>
               </c:pt>
               <c:pt idx="22">
-                <c:v>2.2001719999999998</c:v>
+                <c:v>6.3726660000000004E-2</c:v>
               </c:pt>
               <c:pt idx="23">
-                <c:v>1.8740159999999999</c:v>
+                <c:v>5.4279750000000002E-2</c:v>
               </c:pt>
               <c:pt idx="24">
-                <c:v>1.5973740000000001</c:v>
+                <c:v>4.6266969999999998E-2</c:v>
               </c:pt>
               <c:pt idx="25">
-                <c:v>1.3625579999999999</c:v>
+                <c:v>3.9465680000000003E-2</c:v>
               </c:pt>
               <c:pt idx="26">
-                <c:v>1.163089</c:v>
+                <c:v>3.3688170000000003E-2</c:v>
               </c:pt>
               <c:pt idx="27">
-                <c:v>0.99352839999999998</c:v>
+                <c:v>2.8776949999999999E-2</c:v>
               </c:pt>
               <c:pt idx="28">
-                <c:v>0.84928090000000001</c:v>
+                <c:v>2.4598910000000002E-2</c:v>
               </c:pt>
               <c:pt idx="29">
-                <c:v>0.72648230000000003</c:v>
+                <c:v>2.1042129999999999E-2</c:v>
               </c:pt>
               <c:pt idx="30">
-                <c:v>0.62187110000000001</c:v>
+                <c:v>1.801212E-2</c:v>
               </c:pt>
               <c:pt idx="31">
-                <c:v>0.53268590000000005</c:v>
+                <c:v>1.542893E-2</c:v>
               </c:pt>
               <c:pt idx="32">
-                <c:v>0.45658749999999998</c:v>
+                <c:v>1.322478E-2</c:v>
               </c:pt>
               <c:pt idx="33">
-                <c:v>0.3888161</c:v>
+                <c:v>1.1261820000000001E-2</c:v>
               </c:pt>
               <c:pt idx="34">
-                <c:v>0.33174389999999998</c:v>
+                <c:v>9.6087610000000004E-3</c:v>
               </c:pt>
               <c:pt idx="35">
-                <c:v>0.28358420000000001</c:v>
+                <c:v>8.2138449999999991E-3</c:v>
               </c:pt>
               <c:pt idx="36">
-                <c:v>0.24286250000000001</c:v>
+                <c:v>7.0343660000000002E-3</c:v>
               </c:pt>
               <c:pt idx="37">
-                <c:v>0.20836250000000001</c:v>
+                <c:v>6.0350960000000002E-3</c:v>
               </c:pt>
               <c:pt idx="38">
-                <c:v>0.1790783</c:v>
+                <c:v>5.1868940000000001E-3</c:v>
               </c:pt>
               <c:pt idx="39">
-                <c:v>0.15417439999999999</c:v>
+                <c:v>4.4655679999999996E-3</c:v>
               </c:pt>
               <c:pt idx="40">
-                <c:v>0.13295689999999999</c:v>
+                <c:v>3.8510179999999999E-3</c:v>
               </c:pt>
               <c:pt idx="41">
-                <c:v>0.1148479</c:v>
+                <c:v>3.3265E-3</c:v>
               </c:pt>
               <c:pt idx="42">
-                <c:v>9.9364759999999996E-2</c:v>
+                <c:v>2.878041E-3</c:v>
               </c:pt>
               <c:pt idx="43">
-                <c:v>8.6104189999999997E-2</c:v>
+                <c:v>2.4939559999999999E-3</c:v>
               </c:pt>
               <c:pt idx="44">
-                <c:v>7.4728000000000003E-2</c:v>
+                <c:v>2.1644519999999999E-3</c:v>
               </c:pt>
               <c:pt idx="45">
-                <c:v>6.4952609999999994E-2</c:v>
+                <c:v>1.8813129999999999E-3</c:v>
               </c:pt>
               <c:pt idx="46">
-                <c:v>5.6539279999999997E-2</c:v>
+                <c:v>1.6376260000000001E-3</c:v>
               </c:pt>
               <c:pt idx="47">
-                <c:v>4.9284790000000002E-2</c:v>
+                <c:v>1.4275049999999999E-3</c:v>
               </c:pt>
               <c:pt idx="48">
-                <c:v>4.344046E-2</c:v>
+                <c:v>1.258227E-3</c:v>
               </c:pt>
               <c:pt idx="49">
-                <c:v>3.8289160000000003E-2</c:v>
+                <c:v>1.109023E-3</c:v>
               </c:pt>
               <c:pt idx="50">
-                <c:v>3.3748720000000003E-2</c:v>
+                <c:v>9.7751159999999991E-4</c:v>
               </c:pt>
               <c:pt idx="51">
-                <c:v>2.9746539999999998E-2</c:v>
+                <c:v>8.6159080000000002E-4</c:v>
               </c:pt>
               <c:pt idx="52">
-                <c:v>2.6475800000000001E-2</c:v>
+                <c:v>7.6685580000000004E-4</c:v>
               </c:pt>
               <c:pt idx="53">
-                <c:v>2.3535819999999999E-2</c:v>
+                <c:v>6.8170079999999998E-4</c:v>
               </c:pt>
               <c:pt idx="54">
-                <c:v>2.0896209999999998E-2</c:v>
+                <c:v>6.0524609999999996E-4</c:v>
               </c:pt>
               <c:pt idx="55">
-                <c:v>1.8528929999999999E-2</c:v>
+                <c:v>5.3667929999999997E-4</c:v>
               </c:pt>
               <c:pt idx="56">
-                <c:v>1.640844E-2</c:v>
+                <c:v>4.7526069999999999E-4</c:v>
               </c:pt>
               <c:pt idx="57">
-                <c:v>1.451125E-2</c:v>
+                <c:v>4.2030950000000001E-4</c:v>
               </c:pt>
               <c:pt idx="58">
-                <c:v>1.281594E-2</c:v>
+                <c:v>3.7120600000000001E-4</c:v>
               </c:pt>
               <c:pt idx="59">
-                <c:v>1.1302939999999999E-2</c:v>
-              </c:pt>
-              <c:pt idx="60">
-                <c:v>9.9543470000000005E-3</c:v>
-              </c:pt>
-              <c:pt idx="61">
-                <c:v>8.7538979999999995E-3</c:v>
+                <c:v>0</c:v>
               </c:pt>
             </c:numLit>
           </c:val>
@@ -5951,7 +6104,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" saveData="0" refreshedBy="Daniel Lodholm" refreshedDate="44929.758118171296" backgroundQuery="1" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1" xr:uid="{C4B3B5B2-8205-4863-A006-53D4544A734E}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" saveData="0" refreshedBy="Daniel Lodholm" refreshedDate="45283.81659722222" backgroundQuery="1" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1" xr:uid="{4DCD81BD-52B0-4A5F-AB33-A7B1F909D6A5}">
   <cacheSource type="external" connectionId="2">
     <extLst>
       <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{F057638F-6D5F-4e77-A914-E7F072B9BCA8}">
@@ -5961,7 +6114,7 @@
   </cacheSource>
   <cacheFields count="2">
     <cacheField name="[testoutput].[Altitude].[Altitude]" caption="Altitude" numFmtId="0" level="1">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="0" maxValue="61000" count="62">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="0" maxValue="59000" count="60">
         <n v="0"/>
         <n v="1000"/>
         <n v="2000"/>
@@ -6022,8 +6175,6 @@
         <n v="57000"/>
         <n v="58000"/>
         <n v="59000"/>
-        <n v="60000"/>
-        <n v="61000"/>
       </sharedItems>
       <extLst>
         <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{4F2E5C28-24EA-4eb8-9CBF-B6C8F9C3D259}">
@@ -6088,8 +6239,422 @@
             <x15:cachedUniqueName index="57" name="[testoutput].[Altitude].&amp;[57000]"/>
             <x15:cachedUniqueName index="58" name="[testoutput].[Altitude].&amp;[58000]"/>
             <x15:cachedUniqueName index="59" name="[testoutput].[Altitude].&amp;[59000]"/>
-            <x15:cachedUniqueName index="60" name="[testoutput].[Altitude].&amp;[60000]"/>
-            <x15:cachedUniqueName index="61" name="[testoutput].[Altitude].&amp;[61000]"/>
+          </x15:cachedUniqueNames>
+        </ext>
+      </extLst>
+    </cacheField>
+    <cacheField name="[Measures].[Sum of Density]" caption="Sum of Density" numFmtId="0" hierarchy="8" level="32767"/>
+  </cacheFields>
+  <cacheHierarchies count="10">
+    <cacheHierarchy uniqueName="[testoutput].[Altitude]" caption="Altitude" attribute="1" defaultMemberUniqueName="[testoutput].[Altitude].[All]" allUniqueName="[testoutput].[Altitude].[All]" dimensionUniqueName="[testoutput]" displayFolder="" count="2" memberValueDatatype="20" unbalanced="0">
+      <fieldsUsage count="2">
+        <fieldUsage x="-1"/>
+        <fieldUsage x="0"/>
+      </fieldsUsage>
+    </cacheHierarchy>
+    <cacheHierarchy uniqueName="[testoutput].[Temperature]" caption="Temperature" attribute="1" defaultMemberUniqueName="[testoutput].[Temperature].[All]" allUniqueName="[testoutput].[Temperature].[All]" dimensionUniqueName="[testoutput]" displayFolder="" count="0" memberValueDatatype="5" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[testoutput].[Pressure]" caption="Pressure" attribute="1" defaultMemberUniqueName="[testoutput].[Pressure].[All]" allUniqueName="[testoutput].[Pressure].[All]" dimensionUniqueName="[testoutput]" displayFolder="" count="0" memberValueDatatype="5" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[testoutput].[Density]" caption="Density" attribute="1" defaultMemberUniqueName="[testoutput].[Density].[All]" allUniqueName="[testoutput].[Density].[All]" dimensionUniqueName="[testoutput]" displayFolder="" count="0" memberValueDatatype="5" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Measures].[__XL_Count testoutput]" caption="__XL_Count testoutput" measure="1" displayFolder="" measureGroup="testoutput" count="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Measures].[__No measures defined]" caption="__No measures defined" measure="1" displayFolder="" count="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Measures].[Sum of Temperature]" caption="Sum of Temperature" measure="1" displayFolder="" measureGroup="testoutput" count="0" hidden="1">
+      <extLst>
+        <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{B97F6D7D-B522-45F9-BDA1-12C45D357490}">
+          <x15:cacheHierarchy aggregatedColumn="1"/>
+        </ext>
+      </extLst>
+    </cacheHierarchy>
+    <cacheHierarchy uniqueName="[Measures].[Sum of Pressure]" caption="Sum of Pressure" measure="1" displayFolder="" measureGroup="testoutput" count="0" hidden="1">
+      <extLst>
+        <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{B97F6D7D-B522-45F9-BDA1-12C45D357490}">
+          <x15:cacheHierarchy aggregatedColumn="2"/>
+        </ext>
+      </extLst>
+    </cacheHierarchy>
+    <cacheHierarchy uniqueName="[Measures].[Sum of Density]" caption="Sum of Density" measure="1" displayFolder="" measureGroup="testoutput" count="0" oneField="1" hidden="1">
+      <fieldsUsage count="1">
+        <fieldUsage x="1"/>
+      </fieldsUsage>
+      <extLst>
+        <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{B97F6D7D-B522-45F9-BDA1-12C45D357490}">
+          <x15:cacheHierarchy aggregatedColumn="3"/>
+        </ext>
+      </extLst>
+    </cacheHierarchy>
+    <cacheHierarchy uniqueName="[Measures].[Sum of Altitude]" caption="Sum of Altitude" measure="1" displayFolder="" measureGroup="testoutput" count="0" hidden="1">
+      <extLst>
+        <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{B97F6D7D-B522-45F9-BDA1-12C45D357490}">
+          <x15:cacheHierarchy aggregatedColumn="0"/>
+        </ext>
+      </extLst>
+    </cacheHierarchy>
+  </cacheHierarchies>
+  <kpis count="0"/>
+  <dimensions count="2">
+    <dimension measure="1" name="Measures" uniqueName="[Measures]" caption="Measures"/>
+    <dimension name="testoutput" uniqueName="[testoutput]" caption="testoutput"/>
+  </dimensions>
+  <measureGroups count="1">
+    <measureGroup name="testoutput" caption="testoutput"/>
+  </measureGroups>
+  <maps count="1">
+    <map measureGroup="0" dimension="1"/>
+  </maps>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition pivotCacheId="806323974" supportSubqueryNonVisual="1" supportSubqueryCalcMem="1" supportAddCalcMems="1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{ABF5C744-AB39-4b91-8756-CFA1BBC848D5}">
+      <x15:pivotCacheIdVersion cacheIdSupportedVersion="6" cacheIdCreatedVersion="7"/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheDefinition2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" saveData="0" refreshedBy="Daniel Lodholm" refreshedDate="45283.816598263889" backgroundQuery="1" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1" xr:uid="{B70AC161-DA3C-445E-9C44-66A01B49AFC4}">
+  <cacheSource type="external" connectionId="2">
+    <extLst>
+      <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{F057638F-6D5F-4e77-A914-E7F072B9BCA8}">
+        <x14:sourceConnection name="ThisWorkbookDataModel"/>
+      </ext>
+    </extLst>
+  </cacheSource>
+  <cacheFields count="2">
+    <cacheField name="[testoutput].[Altitude].[Altitude]" caption="Altitude" numFmtId="0" level="1">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="0" maxValue="59000" count="60">
+        <n v="0"/>
+        <n v="1000"/>
+        <n v="2000"/>
+        <n v="3000"/>
+        <n v="4000"/>
+        <n v="5000"/>
+        <n v="6000"/>
+        <n v="7000"/>
+        <n v="8000"/>
+        <n v="9000"/>
+        <n v="10000"/>
+        <n v="11000"/>
+        <n v="12000"/>
+        <n v="13000"/>
+        <n v="14000"/>
+        <n v="15000"/>
+        <n v="16000"/>
+        <n v="17000"/>
+        <n v="18000"/>
+        <n v="19000"/>
+        <n v="20000"/>
+        <n v="21000"/>
+        <n v="22000"/>
+        <n v="23000"/>
+        <n v="24000"/>
+        <n v="25000"/>
+        <n v="26000"/>
+        <n v="27000"/>
+        <n v="28000"/>
+        <n v="29000"/>
+        <n v="30000"/>
+        <n v="31000"/>
+        <n v="32000"/>
+        <n v="33000"/>
+        <n v="34000"/>
+        <n v="35000"/>
+        <n v="36000"/>
+        <n v="37000"/>
+        <n v="38000"/>
+        <n v="39000"/>
+        <n v="40000"/>
+        <n v="41000"/>
+        <n v="42000"/>
+        <n v="43000"/>
+        <n v="44000"/>
+        <n v="45000"/>
+        <n v="46000"/>
+        <n v="47000"/>
+        <n v="48000"/>
+        <n v="49000"/>
+        <n v="50000"/>
+        <n v="51000"/>
+        <n v="52000"/>
+        <n v="53000"/>
+        <n v="54000"/>
+        <n v="55000"/>
+        <n v="56000"/>
+        <n v="57000"/>
+        <n v="58000"/>
+        <n v="59000"/>
+      </sharedItems>
+      <extLst>
+        <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{4F2E5C28-24EA-4eb8-9CBF-B6C8F9C3D259}">
+          <x15:cachedUniqueNames>
+            <x15:cachedUniqueName index="0" name="[testoutput].[Altitude].&amp;[0]"/>
+            <x15:cachedUniqueName index="1" name="[testoutput].[Altitude].&amp;[1000]"/>
+            <x15:cachedUniqueName index="2" name="[testoutput].[Altitude].&amp;[2000]"/>
+            <x15:cachedUniqueName index="3" name="[testoutput].[Altitude].&amp;[3000]"/>
+            <x15:cachedUniqueName index="4" name="[testoutput].[Altitude].&amp;[4000]"/>
+            <x15:cachedUniqueName index="5" name="[testoutput].[Altitude].&amp;[5000]"/>
+            <x15:cachedUniqueName index="6" name="[testoutput].[Altitude].&amp;[6000]"/>
+            <x15:cachedUniqueName index="7" name="[testoutput].[Altitude].&amp;[7000]"/>
+            <x15:cachedUniqueName index="8" name="[testoutput].[Altitude].&amp;[8000]"/>
+            <x15:cachedUniqueName index="9" name="[testoutput].[Altitude].&amp;[9000]"/>
+            <x15:cachedUniqueName index="10" name="[testoutput].[Altitude].&amp;[10000]"/>
+            <x15:cachedUniqueName index="11" name="[testoutput].[Altitude].&amp;[11000]"/>
+            <x15:cachedUniqueName index="12" name="[testoutput].[Altitude].&amp;[12000]"/>
+            <x15:cachedUniqueName index="13" name="[testoutput].[Altitude].&amp;[13000]"/>
+            <x15:cachedUniqueName index="14" name="[testoutput].[Altitude].&amp;[14000]"/>
+            <x15:cachedUniqueName index="15" name="[testoutput].[Altitude].&amp;[15000]"/>
+            <x15:cachedUniqueName index="16" name="[testoutput].[Altitude].&amp;[16000]"/>
+            <x15:cachedUniqueName index="17" name="[testoutput].[Altitude].&amp;[17000]"/>
+            <x15:cachedUniqueName index="18" name="[testoutput].[Altitude].&amp;[18000]"/>
+            <x15:cachedUniqueName index="19" name="[testoutput].[Altitude].&amp;[19000]"/>
+            <x15:cachedUniqueName index="20" name="[testoutput].[Altitude].&amp;[20000]"/>
+            <x15:cachedUniqueName index="21" name="[testoutput].[Altitude].&amp;[21000]"/>
+            <x15:cachedUniqueName index="22" name="[testoutput].[Altitude].&amp;[22000]"/>
+            <x15:cachedUniqueName index="23" name="[testoutput].[Altitude].&amp;[23000]"/>
+            <x15:cachedUniqueName index="24" name="[testoutput].[Altitude].&amp;[24000]"/>
+            <x15:cachedUniqueName index="25" name="[testoutput].[Altitude].&amp;[25000]"/>
+            <x15:cachedUniqueName index="26" name="[testoutput].[Altitude].&amp;[26000]"/>
+            <x15:cachedUniqueName index="27" name="[testoutput].[Altitude].&amp;[27000]"/>
+            <x15:cachedUniqueName index="28" name="[testoutput].[Altitude].&amp;[28000]"/>
+            <x15:cachedUniqueName index="29" name="[testoutput].[Altitude].&amp;[29000]"/>
+            <x15:cachedUniqueName index="30" name="[testoutput].[Altitude].&amp;[30000]"/>
+            <x15:cachedUniqueName index="31" name="[testoutput].[Altitude].&amp;[31000]"/>
+            <x15:cachedUniqueName index="32" name="[testoutput].[Altitude].&amp;[32000]"/>
+            <x15:cachedUniqueName index="33" name="[testoutput].[Altitude].&amp;[33000]"/>
+            <x15:cachedUniqueName index="34" name="[testoutput].[Altitude].&amp;[34000]"/>
+            <x15:cachedUniqueName index="35" name="[testoutput].[Altitude].&amp;[35000]"/>
+            <x15:cachedUniqueName index="36" name="[testoutput].[Altitude].&amp;[36000]"/>
+            <x15:cachedUniqueName index="37" name="[testoutput].[Altitude].&amp;[37000]"/>
+            <x15:cachedUniqueName index="38" name="[testoutput].[Altitude].&amp;[38000]"/>
+            <x15:cachedUniqueName index="39" name="[testoutput].[Altitude].&amp;[39000]"/>
+            <x15:cachedUniqueName index="40" name="[testoutput].[Altitude].&amp;[40000]"/>
+            <x15:cachedUniqueName index="41" name="[testoutput].[Altitude].&amp;[41000]"/>
+            <x15:cachedUniqueName index="42" name="[testoutput].[Altitude].&amp;[42000]"/>
+            <x15:cachedUniqueName index="43" name="[testoutput].[Altitude].&amp;[43000]"/>
+            <x15:cachedUniqueName index="44" name="[testoutput].[Altitude].&amp;[44000]"/>
+            <x15:cachedUniqueName index="45" name="[testoutput].[Altitude].&amp;[45000]"/>
+            <x15:cachedUniqueName index="46" name="[testoutput].[Altitude].&amp;[46000]"/>
+            <x15:cachedUniqueName index="47" name="[testoutput].[Altitude].&amp;[47000]"/>
+            <x15:cachedUniqueName index="48" name="[testoutput].[Altitude].&amp;[48000]"/>
+            <x15:cachedUniqueName index="49" name="[testoutput].[Altitude].&amp;[49000]"/>
+            <x15:cachedUniqueName index="50" name="[testoutput].[Altitude].&amp;[50000]"/>
+            <x15:cachedUniqueName index="51" name="[testoutput].[Altitude].&amp;[51000]"/>
+            <x15:cachedUniqueName index="52" name="[testoutput].[Altitude].&amp;[52000]"/>
+            <x15:cachedUniqueName index="53" name="[testoutput].[Altitude].&amp;[53000]"/>
+            <x15:cachedUniqueName index="54" name="[testoutput].[Altitude].&amp;[54000]"/>
+            <x15:cachedUniqueName index="55" name="[testoutput].[Altitude].&amp;[55000]"/>
+            <x15:cachedUniqueName index="56" name="[testoutput].[Altitude].&amp;[56000]"/>
+            <x15:cachedUniqueName index="57" name="[testoutput].[Altitude].&amp;[57000]"/>
+            <x15:cachedUniqueName index="58" name="[testoutput].[Altitude].&amp;[58000]"/>
+            <x15:cachedUniqueName index="59" name="[testoutput].[Altitude].&amp;[59000]"/>
+          </x15:cachedUniqueNames>
+        </ext>
+      </extLst>
+    </cacheField>
+    <cacheField name="[Measures].[Sum of Pressure]" caption="Sum of Pressure" numFmtId="0" hierarchy="7" level="32767"/>
+  </cacheFields>
+  <cacheHierarchies count="10">
+    <cacheHierarchy uniqueName="[testoutput].[Altitude]" caption="Altitude" attribute="1" defaultMemberUniqueName="[testoutput].[Altitude].[All]" allUniqueName="[testoutput].[Altitude].[All]" dimensionUniqueName="[testoutput]" displayFolder="" count="2" memberValueDatatype="20" unbalanced="0">
+      <fieldsUsage count="2">
+        <fieldUsage x="-1"/>
+        <fieldUsage x="0"/>
+      </fieldsUsage>
+    </cacheHierarchy>
+    <cacheHierarchy uniqueName="[testoutput].[Temperature]" caption="Temperature" attribute="1" defaultMemberUniqueName="[testoutput].[Temperature].[All]" allUniqueName="[testoutput].[Temperature].[All]" dimensionUniqueName="[testoutput]" displayFolder="" count="0" memberValueDatatype="5" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[testoutput].[Pressure]" caption="Pressure" attribute="1" defaultMemberUniqueName="[testoutput].[Pressure].[All]" allUniqueName="[testoutput].[Pressure].[All]" dimensionUniqueName="[testoutput]" displayFolder="" count="0" memberValueDatatype="5" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[testoutput].[Density]" caption="Density" attribute="1" defaultMemberUniqueName="[testoutput].[Density].[All]" allUniqueName="[testoutput].[Density].[All]" dimensionUniqueName="[testoutput]" displayFolder="" count="0" memberValueDatatype="5" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Measures].[__XL_Count testoutput]" caption="__XL_Count testoutput" measure="1" displayFolder="" measureGroup="testoutput" count="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Measures].[__No measures defined]" caption="__No measures defined" measure="1" displayFolder="" count="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Measures].[Sum of Temperature]" caption="Sum of Temperature" measure="1" displayFolder="" measureGroup="testoutput" count="0" hidden="1">
+      <extLst>
+        <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{B97F6D7D-B522-45F9-BDA1-12C45D357490}">
+          <x15:cacheHierarchy aggregatedColumn="1"/>
+        </ext>
+      </extLst>
+    </cacheHierarchy>
+    <cacheHierarchy uniqueName="[Measures].[Sum of Pressure]" caption="Sum of Pressure" measure="1" displayFolder="" measureGroup="testoutput" count="0" oneField="1" hidden="1">
+      <fieldsUsage count="1">
+        <fieldUsage x="1"/>
+      </fieldsUsage>
+      <extLst>
+        <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{B97F6D7D-B522-45F9-BDA1-12C45D357490}">
+          <x15:cacheHierarchy aggregatedColumn="2"/>
+        </ext>
+      </extLst>
+    </cacheHierarchy>
+    <cacheHierarchy uniqueName="[Measures].[Sum of Density]" caption="Sum of Density" measure="1" displayFolder="" measureGroup="testoutput" count="0" hidden="1">
+      <extLst>
+        <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{B97F6D7D-B522-45F9-BDA1-12C45D357490}">
+          <x15:cacheHierarchy aggregatedColumn="3"/>
+        </ext>
+      </extLst>
+    </cacheHierarchy>
+    <cacheHierarchy uniqueName="[Measures].[Sum of Altitude]" caption="Sum of Altitude" measure="1" displayFolder="" measureGroup="testoutput" count="0" hidden="1">
+      <extLst>
+        <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{B97F6D7D-B522-45F9-BDA1-12C45D357490}">
+          <x15:cacheHierarchy aggregatedColumn="0"/>
+        </ext>
+      </extLst>
+    </cacheHierarchy>
+  </cacheHierarchies>
+  <kpis count="0"/>
+  <dimensions count="2">
+    <dimension measure="1" name="Measures" uniqueName="[Measures]" caption="Measures"/>
+    <dimension name="testoutput" uniqueName="[testoutput]" caption="testoutput"/>
+  </dimensions>
+  <measureGroups count="1">
+    <measureGroup name="testoutput" caption="testoutput"/>
+  </measureGroups>
+  <maps count="1">
+    <map measureGroup="0" dimension="1"/>
+  </maps>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition pivotCacheId="502512662" supportSubqueryNonVisual="1" supportSubqueryCalcMem="1" supportAddCalcMems="1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{ABF5C744-AB39-4b91-8756-CFA1BBC848D5}">
+      <x15:pivotCacheIdVersion cacheIdSupportedVersion="6" cacheIdCreatedVersion="7"/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheDefinition3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" saveData="0" refreshedBy="Daniel Lodholm" refreshedDate="45283.816599421298" backgroundQuery="1" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1" xr:uid="{C4B3B5B2-8205-4863-A006-53D4544A734E}">
+  <cacheSource type="external" connectionId="2">
+    <extLst>
+      <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{F057638F-6D5F-4e77-A914-E7F072B9BCA8}">
+        <x14:sourceConnection name="ThisWorkbookDataModel"/>
+      </ext>
+    </extLst>
+  </cacheSource>
+  <cacheFields count="2">
+    <cacheField name="[testoutput].[Altitude].[Altitude]" caption="Altitude" numFmtId="0" level="1">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="0" maxValue="59000" count="60">
+        <n v="0"/>
+        <n v="1000"/>
+        <n v="2000"/>
+        <n v="3000"/>
+        <n v="4000"/>
+        <n v="5000"/>
+        <n v="6000"/>
+        <n v="7000"/>
+        <n v="8000"/>
+        <n v="9000"/>
+        <n v="10000"/>
+        <n v="11000"/>
+        <n v="12000"/>
+        <n v="13000"/>
+        <n v="14000"/>
+        <n v="15000"/>
+        <n v="16000"/>
+        <n v="17000"/>
+        <n v="18000"/>
+        <n v="19000"/>
+        <n v="20000"/>
+        <n v="21000"/>
+        <n v="22000"/>
+        <n v="23000"/>
+        <n v="24000"/>
+        <n v="25000"/>
+        <n v="26000"/>
+        <n v="27000"/>
+        <n v="28000"/>
+        <n v="29000"/>
+        <n v="30000"/>
+        <n v="31000"/>
+        <n v="32000"/>
+        <n v="33000"/>
+        <n v="34000"/>
+        <n v="35000"/>
+        <n v="36000"/>
+        <n v="37000"/>
+        <n v="38000"/>
+        <n v="39000"/>
+        <n v="40000"/>
+        <n v="41000"/>
+        <n v="42000"/>
+        <n v="43000"/>
+        <n v="44000"/>
+        <n v="45000"/>
+        <n v="46000"/>
+        <n v="47000"/>
+        <n v="48000"/>
+        <n v="49000"/>
+        <n v="50000"/>
+        <n v="51000"/>
+        <n v="52000"/>
+        <n v="53000"/>
+        <n v="54000"/>
+        <n v="55000"/>
+        <n v="56000"/>
+        <n v="57000"/>
+        <n v="58000"/>
+        <n v="59000"/>
+      </sharedItems>
+      <extLst>
+        <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{4F2E5C28-24EA-4eb8-9CBF-B6C8F9C3D259}">
+          <x15:cachedUniqueNames>
+            <x15:cachedUniqueName index="0" name="[testoutput].[Altitude].&amp;[0]"/>
+            <x15:cachedUniqueName index="1" name="[testoutput].[Altitude].&amp;[1000]"/>
+            <x15:cachedUniqueName index="2" name="[testoutput].[Altitude].&amp;[2000]"/>
+            <x15:cachedUniqueName index="3" name="[testoutput].[Altitude].&amp;[3000]"/>
+            <x15:cachedUniqueName index="4" name="[testoutput].[Altitude].&amp;[4000]"/>
+            <x15:cachedUniqueName index="5" name="[testoutput].[Altitude].&amp;[5000]"/>
+            <x15:cachedUniqueName index="6" name="[testoutput].[Altitude].&amp;[6000]"/>
+            <x15:cachedUniqueName index="7" name="[testoutput].[Altitude].&amp;[7000]"/>
+            <x15:cachedUniqueName index="8" name="[testoutput].[Altitude].&amp;[8000]"/>
+            <x15:cachedUniqueName index="9" name="[testoutput].[Altitude].&amp;[9000]"/>
+            <x15:cachedUniqueName index="10" name="[testoutput].[Altitude].&amp;[10000]"/>
+            <x15:cachedUniqueName index="11" name="[testoutput].[Altitude].&amp;[11000]"/>
+            <x15:cachedUniqueName index="12" name="[testoutput].[Altitude].&amp;[12000]"/>
+            <x15:cachedUniqueName index="13" name="[testoutput].[Altitude].&amp;[13000]"/>
+            <x15:cachedUniqueName index="14" name="[testoutput].[Altitude].&amp;[14000]"/>
+            <x15:cachedUniqueName index="15" name="[testoutput].[Altitude].&amp;[15000]"/>
+            <x15:cachedUniqueName index="16" name="[testoutput].[Altitude].&amp;[16000]"/>
+            <x15:cachedUniqueName index="17" name="[testoutput].[Altitude].&amp;[17000]"/>
+            <x15:cachedUniqueName index="18" name="[testoutput].[Altitude].&amp;[18000]"/>
+            <x15:cachedUniqueName index="19" name="[testoutput].[Altitude].&amp;[19000]"/>
+            <x15:cachedUniqueName index="20" name="[testoutput].[Altitude].&amp;[20000]"/>
+            <x15:cachedUniqueName index="21" name="[testoutput].[Altitude].&amp;[21000]"/>
+            <x15:cachedUniqueName index="22" name="[testoutput].[Altitude].&amp;[22000]"/>
+            <x15:cachedUniqueName index="23" name="[testoutput].[Altitude].&amp;[23000]"/>
+            <x15:cachedUniqueName index="24" name="[testoutput].[Altitude].&amp;[24000]"/>
+            <x15:cachedUniqueName index="25" name="[testoutput].[Altitude].&amp;[25000]"/>
+            <x15:cachedUniqueName index="26" name="[testoutput].[Altitude].&amp;[26000]"/>
+            <x15:cachedUniqueName index="27" name="[testoutput].[Altitude].&amp;[27000]"/>
+            <x15:cachedUniqueName index="28" name="[testoutput].[Altitude].&amp;[28000]"/>
+            <x15:cachedUniqueName index="29" name="[testoutput].[Altitude].&amp;[29000]"/>
+            <x15:cachedUniqueName index="30" name="[testoutput].[Altitude].&amp;[30000]"/>
+            <x15:cachedUniqueName index="31" name="[testoutput].[Altitude].&amp;[31000]"/>
+            <x15:cachedUniqueName index="32" name="[testoutput].[Altitude].&amp;[32000]"/>
+            <x15:cachedUniqueName index="33" name="[testoutput].[Altitude].&amp;[33000]"/>
+            <x15:cachedUniqueName index="34" name="[testoutput].[Altitude].&amp;[34000]"/>
+            <x15:cachedUniqueName index="35" name="[testoutput].[Altitude].&amp;[35000]"/>
+            <x15:cachedUniqueName index="36" name="[testoutput].[Altitude].&amp;[36000]"/>
+            <x15:cachedUniqueName index="37" name="[testoutput].[Altitude].&amp;[37000]"/>
+            <x15:cachedUniqueName index="38" name="[testoutput].[Altitude].&amp;[38000]"/>
+            <x15:cachedUniqueName index="39" name="[testoutput].[Altitude].&amp;[39000]"/>
+            <x15:cachedUniqueName index="40" name="[testoutput].[Altitude].&amp;[40000]"/>
+            <x15:cachedUniqueName index="41" name="[testoutput].[Altitude].&amp;[41000]"/>
+            <x15:cachedUniqueName index="42" name="[testoutput].[Altitude].&amp;[42000]"/>
+            <x15:cachedUniqueName index="43" name="[testoutput].[Altitude].&amp;[43000]"/>
+            <x15:cachedUniqueName index="44" name="[testoutput].[Altitude].&amp;[44000]"/>
+            <x15:cachedUniqueName index="45" name="[testoutput].[Altitude].&amp;[45000]"/>
+            <x15:cachedUniqueName index="46" name="[testoutput].[Altitude].&amp;[46000]"/>
+            <x15:cachedUniqueName index="47" name="[testoutput].[Altitude].&amp;[47000]"/>
+            <x15:cachedUniqueName index="48" name="[testoutput].[Altitude].&amp;[48000]"/>
+            <x15:cachedUniqueName index="49" name="[testoutput].[Altitude].&amp;[49000]"/>
+            <x15:cachedUniqueName index="50" name="[testoutput].[Altitude].&amp;[50000]"/>
+            <x15:cachedUniqueName index="51" name="[testoutput].[Altitude].&amp;[51000]"/>
+            <x15:cachedUniqueName index="52" name="[testoutput].[Altitude].&amp;[52000]"/>
+            <x15:cachedUniqueName index="53" name="[testoutput].[Altitude].&amp;[53000]"/>
+            <x15:cachedUniqueName index="54" name="[testoutput].[Altitude].&amp;[54000]"/>
+            <x15:cachedUniqueName index="55" name="[testoutput].[Altitude].&amp;[55000]"/>
+            <x15:cachedUniqueName index="56" name="[testoutput].[Altitude].&amp;[56000]"/>
+            <x15:cachedUniqueName index="57" name="[testoutput].[Altitude].&amp;[57000]"/>
+            <x15:cachedUniqueName index="58" name="[testoutput].[Altitude].&amp;[58000]"/>
+            <x15:cachedUniqueName index="59" name="[testoutput].[Altitude].&amp;[59000]"/>
           </x15:cachedUniqueNames>
         </ext>
       </extLst>
@@ -6162,436 +6727,12 @@
 </pivotCacheDefinition>
 </file>
 
-<file path=xl/pivotCache/pivotCacheDefinition2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" saveData="0" refreshedBy="Daniel Lodholm" refreshedDate="44929.759325694446" backgroundQuery="1" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1" xr:uid="{B70AC161-DA3C-445E-9C44-66A01B49AFC4}">
-  <cacheSource type="external" connectionId="2">
-    <extLst>
-      <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{F057638F-6D5F-4e77-A914-E7F072B9BCA8}">
-        <x14:sourceConnection name="ThisWorkbookDataModel"/>
-      </ext>
-    </extLst>
-  </cacheSource>
-  <cacheFields count="2">
-    <cacheField name="[testoutput].[Altitude].[Altitude]" caption="Altitude" numFmtId="0" level="1">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="0" maxValue="61000" count="62">
-        <n v="0"/>
-        <n v="1000"/>
-        <n v="2000"/>
-        <n v="3000"/>
-        <n v="4000"/>
-        <n v="5000"/>
-        <n v="6000"/>
-        <n v="7000"/>
-        <n v="8000"/>
-        <n v="9000"/>
-        <n v="10000"/>
-        <n v="11000"/>
-        <n v="12000"/>
-        <n v="13000"/>
-        <n v="14000"/>
-        <n v="15000"/>
-        <n v="16000"/>
-        <n v="17000"/>
-        <n v="18000"/>
-        <n v="19000"/>
-        <n v="20000"/>
-        <n v="21000"/>
-        <n v="22000"/>
-        <n v="23000"/>
-        <n v="24000"/>
-        <n v="25000"/>
-        <n v="26000"/>
-        <n v="27000"/>
-        <n v="28000"/>
-        <n v="29000"/>
-        <n v="30000"/>
-        <n v="31000"/>
-        <n v="32000"/>
-        <n v="33000"/>
-        <n v="34000"/>
-        <n v="35000"/>
-        <n v="36000"/>
-        <n v="37000"/>
-        <n v="38000"/>
-        <n v="39000"/>
-        <n v="40000"/>
-        <n v="41000"/>
-        <n v="42000"/>
-        <n v="43000"/>
-        <n v="44000"/>
-        <n v="45000"/>
-        <n v="46000"/>
-        <n v="47000"/>
-        <n v="48000"/>
-        <n v="49000"/>
-        <n v="50000"/>
-        <n v="51000"/>
-        <n v="52000"/>
-        <n v="53000"/>
-        <n v="54000"/>
-        <n v="55000"/>
-        <n v="56000"/>
-        <n v="57000"/>
-        <n v="58000"/>
-        <n v="59000"/>
-        <n v="60000"/>
-        <n v="61000"/>
-      </sharedItems>
-      <extLst>
-        <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{4F2E5C28-24EA-4eb8-9CBF-B6C8F9C3D259}">
-          <x15:cachedUniqueNames>
-            <x15:cachedUniqueName index="0" name="[testoutput].[Altitude].&amp;[0]"/>
-            <x15:cachedUniqueName index="1" name="[testoutput].[Altitude].&amp;[1000]"/>
-            <x15:cachedUniqueName index="2" name="[testoutput].[Altitude].&amp;[2000]"/>
-            <x15:cachedUniqueName index="3" name="[testoutput].[Altitude].&amp;[3000]"/>
-            <x15:cachedUniqueName index="4" name="[testoutput].[Altitude].&amp;[4000]"/>
-            <x15:cachedUniqueName index="5" name="[testoutput].[Altitude].&amp;[5000]"/>
-            <x15:cachedUniqueName index="6" name="[testoutput].[Altitude].&amp;[6000]"/>
-            <x15:cachedUniqueName index="7" name="[testoutput].[Altitude].&amp;[7000]"/>
-            <x15:cachedUniqueName index="8" name="[testoutput].[Altitude].&amp;[8000]"/>
-            <x15:cachedUniqueName index="9" name="[testoutput].[Altitude].&amp;[9000]"/>
-            <x15:cachedUniqueName index="10" name="[testoutput].[Altitude].&amp;[10000]"/>
-            <x15:cachedUniqueName index="11" name="[testoutput].[Altitude].&amp;[11000]"/>
-            <x15:cachedUniqueName index="12" name="[testoutput].[Altitude].&amp;[12000]"/>
-            <x15:cachedUniqueName index="13" name="[testoutput].[Altitude].&amp;[13000]"/>
-            <x15:cachedUniqueName index="14" name="[testoutput].[Altitude].&amp;[14000]"/>
-            <x15:cachedUniqueName index="15" name="[testoutput].[Altitude].&amp;[15000]"/>
-            <x15:cachedUniqueName index="16" name="[testoutput].[Altitude].&amp;[16000]"/>
-            <x15:cachedUniqueName index="17" name="[testoutput].[Altitude].&amp;[17000]"/>
-            <x15:cachedUniqueName index="18" name="[testoutput].[Altitude].&amp;[18000]"/>
-            <x15:cachedUniqueName index="19" name="[testoutput].[Altitude].&amp;[19000]"/>
-            <x15:cachedUniqueName index="20" name="[testoutput].[Altitude].&amp;[20000]"/>
-            <x15:cachedUniqueName index="21" name="[testoutput].[Altitude].&amp;[21000]"/>
-            <x15:cachedUniqueName index="22" name="[testoutput].[Altitude].&amp;[22000]"/>
-            <x15:cachedUniqueName index="23" name="[testoutput].[Altitude].&amp;[23000]"/>
-            <x15:cachedUniqueName index="24" name="[testoutput].[Altitude].&amp;[24000]"/>
-            <x15:cachedUniqueName index="25" name="[testoutput].[Altitude].&amp;[25000]"/>
-            <x15:cachedUniqueName index="26" name="[testoutput].[Altitude].&amp;[26000]"/>
-            <x15:cachedUniqueName index="27" name="[testoutput].[Altitude].&amp;[27000]"/>
-            <x15:cachedUniqueName index="28" name="[testoutput].[Altitude].&amp;[28000]"/>
-            <x15:cachedUniqueName index="29" name="[testoutput].[Altitude].&amp;[29000]"/>
-            <x15:cachedUniqueName index="30" name="[testoutput].[Altitude].&amp;[30000]"/>
-            <x15:cachedUniqueName index="31" name="[testoutput].[Altitude].&amp;[31000]"/>
-            <x15:cachedUniqueName index="32" name="[testoutput].[Altitude].&amp;[32000]"/>
-            <x15:cachedUniqueName index="33" name="[testoutput].[Altitude].&amp;[33000]"/>
-            <x15:cachedUniqueName index="34" name="[testoutput].[Altitude].&amp;[34000]"/>
-            <x15:cachedUniqueName index="35" name="[testoutput].[Altitude].&amp;[35000]"/>
-            <x15:cachedUniqueName index="36" name="[testoutput].[Altitude].&amp;[36000]"/>
-            <x15:cachedUniqueName index="37" name="[testoutput].[Altitude].&amp;[37000]"/>
-            <x15:cachedUniqueName index="38" name="[testoutput].[Altitude].&amp;[38000]"/>
-            <x15:cachedUniqueName index="39" name="[testoutput].[Altitude].&amp;[39000]"/>
-            <x15:cachedUniqueName index="40" name="[testoutput].[Altitude].&amp;[40000]"/>
-            <x15:cachedUniqueName index="41" name="[testoutput].[Altitude].&amp;[41000]"/>
-            <x15:cachedUniqueName index="42" name="[testoutput].[Altitude].&amp;[42000]"/>
-            <x15:cachedUniqueName index="43" name="[testoutput].[Altitude].&amp;[43000]"/>
-            <x15:cachedUniqueName index="44" name="[testoutput].[Altitude].&amp;[44000]"/>
-            <x15:cachedUniqueName index="45" name="[testoutput].[Altitude].&amp;[45000]"/>
-            <x15:cachedUniqueName index="46" name="[testoutput].[Altitude].&amp;[46000]"/>
-            <x15:cachedUniqueName index="47" name="[testoutput].[Altitude].&amp;[47000]"/>
-            <x15:cachedUniqueName index="48" name="[testoutput].[Altitude].&amp;[48000]"/>
-            <x15:cachedUniqueName index="49" name="[testoutput].[Altitude].&amp;[49000]"/>
-            <x15:cachedUniqueName index="50" name="[testoutput].[Altitude].&amp;[50000]"/>
-            <x15:cachedUniqueName index="51" name="[testoutput].[Altitude].&amp;[51000]"/>
-            <x15:cachedUniqueName index="52" name="[testoutput].[Altitude].&amp;[52000]"/>
-            <x15:cachedUniqueName index="53" name="[testoutput].[Altitude].&amp;[53000]"/>
-            <x15:cachedUniqueName index="54" name="[testoutput].[Altitude].&amp;[54000]"/>
-            <x15:cachedUniqueName index="55" name="[testoutput].[Altitude].&amp;[55000]"/>
-            <x15:cachedUniqueName index="56" name="[testoutput].[Altitude].&amp;[56000]"/>
-            <x15:cachedUniqueName index="57" name="[testoutput].[Altitude].&amp;[57000]"/>
-            <x15:cachedUniqueName index="58" name="[testoutput].[Altitude].&amp;[58000]"/>
-            <x15:cachedUniqueName index="59" name="[testoutput].[Altitude].&amp;[59000]"/>
-            <x15:cachedUniqueName index="60" name="[testoutput].[Altitude].&amp;[60000]"/>
-            <x15:cachedUniqueName index="61" name="[testoutput].[Altitude].&amp;[61000]"/>
-          </x15:cachedUniqueNames>
-        </ext>
-      </extLst>
-    </cacheField>
-    <cacheField name="[Measures].[Sum of Pressure]" caption="Sum of Pressure" numFmtId="0" hierarchy="7" level="32767"/>
-  </cacheFields>
-  <cacheHierarchies count="10">
-    <cacheHierarchy uniqueName="[testoutput].[Altitude]" caption="Altitude" attribute="1" defaultMemberUniqueName="[testoutput].[Altitude].[All]" allUniqueName="[testoutput].[Altitude].[All]" dimensionUniqueName="[testoutput]" displayFolder="" count="2" memberValueDatatype="20" unbalanced="0">
-      <fieldsUsage count="2">
-        <fieldUsage x="-1"/>
-        <fieldUsage x="0"/>
-      </fieldsUsage>
-    </cacheHierarchy>
-    <cacheHierarchy uniqueName="[testoutput].[Temperature]" caption="Temperature" attribute="1" defaultMemberUniqueName="[testoutput].[Temperature].[All]" allUniqueName="[testoutput].[Temperature].[All]" dimensionUniqueName="[testoutput]" displayFolder="" count="0" memberValueDatatype="5" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[testoutput].[Pressure]" caption="Pressure" attribute="1" defaultMemberUniqueName="[testoutput].[Pressure].[All]" allUniqueName="[testoutput].[Pressure].[All]" dimensionUniqueName="[testoutput]" displayFolder="" count="2" memberValueDatatype="5" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[testoutput].[Density]" caption="Density" attribute="1" defaultMemberUniqueName="[testoutput].[Density].[All]" allUniqueName="[testoutput].[Density].[All]" dimensionUniqueName="[testoutput]" displayFolder="" count="0" memberValueDatatype="5" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Measures].[__XL_Count testoutput]" caption="__XL_Count testoutput" measure="1" displayFolder="" measureGroup="testoutput" count="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Measures].[__No measures defined]" caption="__No measures defined" measure="1" displayFolder="" count="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Measures].[Sum of Temperature]" caption="Sum of Temperature" measure="1" displayFolder="" measureGroup="testoutput" count="0" hidden="1">
-      <extLst>
-        <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{B97F6D7D-B522-45F9-BDA1-12C45D357490}">
-          <x15:cacheHierarchy aggregatedColumn="1"/>
-        </ext>
-      </extLst>
-    </cacheHierarchy>
-    <cacheHierarchy uniqueName="[Measures].[Sum of Pressure]" caption="Sum of Pressure" measure="1" displayFolder="" measureGroup="testoutput" count="0" oneField="1" hidden="1">
-      <fieldsUsage count="1">
-        <fieldUsage x="1"/>
-      </fieldsUsage>
-      <extLst>
-        <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{B97F6D7D-B522-45F9-BDA1-12C45D357490}">
-          <x15:cacheHierarchy aggregatedColumn="2"/>
-        </ext>
-      </extLst>
-    </cacheHierarchy>
-    <cacheHierarchy uniqueName="[Measures].[Sum of Density]" caption="Sum of Density" measure="1" displayFolder="" measureGroup="testoutput" count="0" hidden="1">
-      <extLst>
-        <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{B97F6D7D-B522-45F9-BDA1-12C45D357490}">
-          <x15:cacheHierarchy aggregatedColumn="3"/>
-        </ext>
-      </extLst>
-    </cacheHierarchy>
-    <cacheHierarchy uniqueName="[Measures].[Sum of Altitude]" caption="Sum of Altitude" measure="1" displayFolder="" measureGroup="testoutput" count="0" hidden="1">
-      <extLst>
-        <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{B97F6D7D-B522-45F9-BDA1-12C45D357490}">
-          <x15:cacheHierarchy aggregatedColumn="0"/>
-        </ext>
-      </extLst>
-    </cacheHierarchy>
-  </cacheHierarchies>
-  <kpis count="0"/>
-  <dimensions count="2">
-    <dimension measure="1" name="Measures" uniqueName="[Measures]" caption="Measures"/>
-    <dimension name="testoutput" uniqueName="[testoutput]" caption="testoutput"/>
-  </dimensions>
-  <measureGroups count="1">
-    <measureGroup name="testoutput" caption="testoutput"/>
-  </measureGroups>
-  <maps count="1">
-    <map measureGroup="0" dimension="1"/>
-  </maps>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
-      <x14:pivotCacheDefinition pivotCacheId="502512662" supportSubqueryNonVisual="1" supportSubqueryCalcMem="1" supportAddCalcMems="1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{ABF5C744-AB39-4b91-8756-CFA1BBC848D5}">
-      <x15:pivotCacheIdVersion cacheIdSupportedVersion="6" cacheIdCreatedVersion="7"/>
-    </ext>
-  </extLst>
-</pivotCacheDefinition>
-</file>
-
-<file path=xl/pivotCache/pivotCacheDefinition3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" saveData="0" refreshedBy="Daniel Lodholm" refreshedDate="44929.759830671297" backgroundQuery="1" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1" xr:uid="{4DCD81BD-52B0-4A5F-AB33-A7B1F909D6A5}">
-  <cacheSource type="external" connectionId="2">
-    <extLst>
-      <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{F057638F-6D5F-4e77-A914-E7F072B9BCA8}">
-        <x14:sourceConnection name="ThisWorkbookDataModel"/>
-      </ext>
-    </extLst>
-  </cacheSource>
-  <cacheFields count="2">
-    <cacheField name="[testoutput].[Altitude].[Altitude]" caption="Altitude" numFmtId="0" level="1">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="0" maxValue="61000" count="62">
-        <n v="0"/>
-        <n v="1000"/>
-        <n v="2000"/>
-        <n v="3000"/>
-        <n v="4000"/>
-        <n v="5000"/>
-        <n v="6000"/>
-        <n v="7000"/>
-        <n v="8000"/>
-        <n v="9000"/>
-        <n v="10000"/>
-        <n v="11000"/>
-        <n v="12000"/>
-        <n v="13000"/>
-        <n v="14000"/>
-        <n v="15000"/>
-        <n v="16000"/>
-        <n v="17000"/>
-        <n v="18000"/>
-        <n v="19000"/>
-        <n v="20000"/>
-        <n v="21000"/>
-        <n v="22000"/>
-        <n v="23000"/>
-        <n v="24000"/>
-        <n v="25000"/>
-        <n v="26000"/>
-        <n v="27000"/>
-        <n v="28000"/>
-        <n v="29000"/>
-        <n v="30000"/>
-        <n v="31000"/>
-        <n v="32000"/>
-        <n v="33000"/>
-        <n v="34000"/>
-        <n v="35000"/>
-        <n v="36000"/>
-        <n v="37000"/>
-        <n v="38000"/>
-        <n v="39000"/>
-        <n v="40000"/>
-        <n v="41000"/>
-        <n v="42000"/>
-        <n v="43000"/>
-        <n v="44000"/>
-        <n v="45000"/>
-        <n v="46000"/>
-        <n v="47000"/>
-        <n v="48000"/>
-        <n v="49000"/>
-        <n v="50000"/>
-        <n v="51000"/>
-        <n v="52000"/>
-        <n v="53000"/>
-        <n v="54000"/>
-        <n v="55000"/>
-        <n v="56000"/>
-        <n v="57000"/>
-        <n v="58000"/>
-        <n v="59000"/>
-        <n v="60000"/>
-        <n v="61000"/>
-      </sharedItems>
-      <extLst>
-        <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{4F2E5C28-24EA-4eb8-9CBF-B6C8F9C3D259}">
-          <x15:cachedUniqueNames>
-            <x15:cachedUniqueName index="0" name="[testoutput].[Altitude].&amp;[0]"/>
-            <x15:cachedUniqueName index="1" name="[testoutput].[Altitude].&amp;[1000]"/>
-            <x15:cachedUniqueName index="2" name="[testoutput].[Altitude].&amp;[2000]"/>
-            <x15:cachedUniqueName index="3" name="[testoutput].[Altitude].&amp;[3000]"/>
-            <x15:cachedUniqueName index="4" name="[testoutput].[Altitude].&amp;[4000]"/>
-            <x15:cachedUniqueName index="5" name="[testoutput].[Altitude].&amp;[5000]"/>
-            <x15:cachedUniqueName index="6" name="[testoutput].[Altitude].&amp;[6000]"/>
-            <x15:cachedUniqueName index="7" name="[testoutput].[Altitude].&amp;[7000]"/>
-            <x15:cachedUniqueName index="8" name="[testoutput].[Altitude].&amp;[8000]"/>
-            <x15:cachedUniqueName index="9" name="[testoutput].[Altitude].&amp;[9000]"/>
-            <x15:cachedUniqueName index="10" name="[testoutput].[Altitude].&amp;[10000]"/>
-            <x15:cachedUniqueName index="11" name="[testoutput].[Altitude].&amp;[11000]"/>
-            <x15:cachedUniqueName index="12" name="[testoutput].[Altitude].&amp;[12000]"/>
-            <x15:cachedUniqueName index="13" name="[testoutput].[Altitude].&amp;[13000]"/>
-            <x15:cachedUniqueName index="14" name="[testoutput].[Altitude].&amp;[14000]"/>
-            <x15:cachedUniqueName index="15" name="[testoutput].[Altitude].&amp;[15000]"/>
-            <x15:cachedUniqueName index="16" name="[testoutput].[Altitude].&amp;[16000]"/>
-            <x15:cachedUniqueName index="17" name="[testoutput].[Altitude].&amp;[17000]"/>
-            <x15:cachedUniqueName index="18" name="[testoutput].[Altitude].&amp;[18000]"/>
-            <x15:cachedUniqueName index="19" name="[testoutput].[Altitude].&amp;[19000]"/>
-            <x15:cachedUniqueName index="20" name="[testoutput].[Altitude].&amp;[20000]"/>
-            <x15:cachedUniqueName index="21" name="[testoutput].[Altitude].&amp;[21000]"/>
-            <x15:cachedUniqueName index="22" name="[testoutput].[Altitude].&amp;[22000]"/>
-            <x15:cachedUniqueName index="23" name="[testoutput].[Altitude].&amp;[23000]"/>
-            <x15:cachedUniqueName index="24" name="[testoutput].[Altitude].&amp;[24000]"/>
-            <x15:cachedUniqueName index="25" name="[testoutput].[Altitude].&amp;[25000]"/>
-            <x15:cachedUniqueName index="26" name="[testoutput].[Altitude].&amp;[26000]"/>
-            <x15:cachedUniqueName index="27" name="[testoutput].[Altitude].&amp;[27000]"/>
-            <x15:cachedUniqueName index="28" name="[testoutput].[Altitude].&amp;[28000]"/>
-            <x15:cachedUniqueName index="29" name="[testoutput].[Altitude].&amp;[29000]"/>
-            <x15:cachedUniqueName index="30" name="[testoutput].[Altitude].&amp;[30000]"/>
-            <x15:cachedUniqueName index="31" name="[testoutput].[Altitude].&amp;[31000]"/>
-            <x15:cachedUniqueName index="32" name="[testoutput].[Altitude].&amp;[32000]"/>
-            <x15:cachedUniqueName index="33" name="[testoutput].[Altitude].&amp;[33000]"/>
-            <x15:cachedUniqueName index="34" name="[testoutput].[Altitude].&amp;[34000]"/>
-            <x15:cachedUniqueName index="35" name="[testoutput].[Altitude].&amp;[35000]"/>
-            <x15:cachedUniqueName index="36" name="[testoutput].[Altitude].&amp;[36000]"/>
-            <x15:cachedUniqueName index="37" name="[testoutput].[Altitude].&amp;[37000]"/>
-            <x15:cachedUniqueName index="38" name="[testoutput].[Altitude].&amp;[38000]"/>
-            <x15:cachedUniqueName index="39" name="[testoutput].[Altitude].&amp;[39000]"/>
-            <x15:cachedUniqueName index="40" name="[testoutput].[Altitude].&amp;[40000]"/>
-            <x15:cachedUniqueName index="41" name="[testoutput].[Altitude].&amp;[41000]"/>
-            <x15:cachedUniqueName index="42" name="[testoutput].[Altitude].&amp;[42000]"/>
-            <x15:cachedUniqueName index="43" name="[testoutput].[Altitude].&amp;[43000]"/>
-            <x15:cachedUniqueName index="44" name="[testoutput].[Altitude].&amp;[44000]"/>
-            <x15:cachedUniqueName index="45" name="[testoutput].[Altitude].&amp;[45000]"/>
-            <x15:cachedUniqueName index="46" name="[testoutput].[Altitude].&amp;[46000]"/>
-            <x15:cachedUniqueName index="47" name="[testoutput].[Altitude].&amp;[47000]"/>
-            <x15:cachedUniqueName index="48" name="[testoutput].[Altitude].&amp;[48000]"/>
-            <x15:cachedUniqueName index="49" name="[testoutput].[Altitude].&amp;[49000]"/>
-            <x15:cachedUniqueName index="50" name="[testoutput].[Altitude].&amp;[50000]"/>
-            <x15:cachedUniqueName index="51" name="[testoutput].[Altitude].&amp;[51000]"/>
-            <x15:cachedUniqueName index="52" name="[testoutput].[Altitude].&amp;[52000]"/>
-            <x15:cachedUniqueName index="53" name="[testoutput].[Altitude].&amp;[53000]"/>
-            <x15:cachedUniqueName index="54" name="[testoutput].[Altitude].&amp;[54000]"/>
-            <x15:cachedUniqueName index="55" name="[testoutput].[Altitude].&amp;[55000]"/>
-            <x15:cachedUniqueName index="56" name="[testoutput].[Altitude].&amp;[56000]"/>
-            <x15:cachedUniqueName index="57" name="[testoutput].[Altitude].&amp;[57000]"/>
-            <x15:cachedUniqueName index="58" name="[testoutput].[Altitude].&amp;[58000]"/>
-            <x15:cachedUniqueName index="59" name="[testoutput].[Altitude].&amp;[59000]"/>
-            <x15:cachedUniqueName index="60" name="[testoutput].[Altitude].&amp;[60000]"/>
-            <x15:cachedUniqueName index="61" name="[testoutput].[Altitude].&amp;[61000]"/>
-          </x15:cachedUniqueNames>
-        </ext>
-      </extLst>
-    </cacheField>
-    <cacheField name="[Measures].[Sum of Density]" caption="Sum of Density" numFmtId="0" hierarchy="8" level="32767"/>
-  </cacheFields>
-  <cacheHierarchies count="10">
-    <cacheHierarchy uniqueName="[testoutput].[Altitude]" caption="Altitude" attribute="1" defaultMemberUniqueName="[testoutput].[Altitude].[All]" allUniqueName="[testoutput].[Altitude].[All]" dimensionUniqueName="[testoutput]" displayFolder="" count="2" memberValueDatatype="20" unbalanced="0">
-      <fieldsUsage count="2">
-        <fieldUsage x="-1"/>
-        <fieldUsage x="0"/>
-      </fieldsUsage>
-    </cacheHierarchy>
-    <cacheHierarchy uniqueName="[testoutput].[Temperature]" caption="Temperature" attribute="1" defaultMemberUniqueName="[testoutput].[Temperature].[All]" allUniqueName="[testoutput].[Temperature].[All]" dimensionUniqueName="[testoutput]" displayFolder="" count="0" memberValueDatatype="5" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[testoutput].[Pressure]" caption="Pressure" attribute="1" defaultMemberUniqueName="[testoutput].[Pressure].[All]" allUniqueName="[testoutput].[Pressure].[All]" dimensionUniqueName="[testoutput]" displayFolder="" count="0" memberValueDatatype="5" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[testoutput].[Density]" caption="Density" attribute="1" defaultMemberUniqueName="[testoutput].[Density].[All]" allUniqueName="[testoutput].[Density].[All]" dimensionUniqueName="[testoutput]" displayFolder="" count="0" memberValueDatatype="5" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Measures].[__XL_Count testoutput]" caption="__XL_Count testoutput" measure="1" displayFolder="" measureGroup="testoutput" count="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Measures].[__No measures defined]" caption="__No measures defined" measure="1" displayFolder="" count="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Measures].[Sum of Temperature]" caption="Sum of Temperature" measure="1" displayFolder="" measureGroup="testoutput" count="0" hidden="1">
-      <extLst>
-        <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{B97F6D7D-B522-45F9-BDA1-12C45D357490}">
-          <x15:cacheHierarchy aggregatedColumn="1"/>
-        </ext>
-      </extLst>
-    </cacheHierarchy>
-    <cacheHierarchy uniqueName="[Measures].[Sum of Pressure]" caption="Sum of Pressure" measure="1" displayFolder="" measureGroup="testoutput" count="0" hidden="1">
-      <extLst>
-        <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{B97F6D7D-B522-45F9-BDA1-12C45D357490}">
-          <x15:cacheHierarchy aggregatedColumn="2"/>
-        </ext>
-      </extLst>
-    </cacheHierarchy>
-    <cacheHierarchy uniqueName="[Measures].[Sum of Density]" caption="Sum of Density" measure="1" displayFolder="" measureGroup="testoutput" count="0" oneField="1" hidden="1">
-      <fieldsUsage count="1">
-        <fieldUsage x="1"/>
-      </fieldsUsage>
-      <extLst>
-        <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{B97F6D7D-B522-45F9-BDA1-12C45D357490}">
-          <x15:cacheHierarchy aggregatedColumn="3"/>
-        </ext>
-      </extLst>
-    </cacheHierarchy>
-    <cacheHierarchy uniqueName="[Measures].[Sum of Altitude]" caption="Sum of Altitude" measure="1" displayFolder="" measureGroup="testoutput" count="0" hidden="1">
-      <extLst>
-        <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{B97F6D7D-B522-45F9-BDA1-12C45D357490}">
-          <x15:cacheHierarchy aggregatedColumn="0"/>
-        </ext>
-      </extLst>
-    </cacheHierarchy>
-  </cacheHierarchies>
-  <kpis count="0"/>
-  <dimensions count="2">
-    <dimension measure="1" name="Measures" uniqueName="[Measures]" caption="Measures"/>
-    <dimension name="testoutput" uniqueName="[testoutput]" caption="testoutput"/>
-  </dimensions>
-  <measureGroups count="1">
-    <measureGroup name="testoutput" caption="testoutput"/>
-  </measureGroups>
-  <maps count="1">
-    <map measureGroup="0" dimension="1"/>
-  </maps>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
-      <x14:pivotCacheDefinition pivotCacheId="806323974" supportSubqueryNonVisual="1" supportSubqueryCalcMem="1" supportAddCalcMems="1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{ABF5C744-AB39-4b91-8756-CFA1BBC848D5}">
-      <x15:pivotCacheIdVersion cacheIdSupportedVersion="6" cacheIdCreatedVersion="7"/>
-    </ext>
-  </extLst>
-</pivotCacheDefinition>
-</file>
-
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E6EBDEBF-0633-40E3-AAE5-FBE9E430F117}" name="PivotChartTable3" cacheId="65" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
-  <location ref="A1:B64" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{DB5B6DDB-B8C0-414A-9782-056CB44D8C3F}" name="PivotChartTable1" cacheId="11" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+  <location ref="A1:B62" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="2">
     <pivotField axis="axisRow" allDrilled="1" subtotalTop="0" showAll="0" dataSourceSort="1" defaultSubtotal="0" defaultAttributeDrillState="1">
-      <items count="62">
+      <items count="60">
         <item x="0"/>
         <item x="1"/>
         <item x="2"/>
@@ -6652,8 +6793,6 @@
         <item x="57"/>
         <item x="58"/>
         <item x="59"/>
-        <item x="60"/>
-        <item x="61"/>
       </items>
     </pivotField>
     <pivotField dataField="1" subtotalTop="0" showAll="0" defaultSubtotal="0"/>
@@ -6661,7 +6800,7 @@
   <rowFields count="1">
     <field x="0"/>
   </rowFields>
-  <rowItems count="63">
+  <rowItems count="61">
     <i>
       <x/>
     </i>
@@ -6841,12 +6980,6 @@
     </i>
     <i>
       <x v="59"/>
-    </i>
-    <i>
-      <x v="60"/>
-    </i>
-    <i>
-      <x v="61"/>
     </i>
     <i t="grand">
       <x/>
@@ -6856,7 +6989,7 @@
     <i/>
   </colItems>
   <dataFields count="1">
-    <dataField name="Density (kg/m^3)" fld="1" baseField="0" baseItem="8"/>
+    <dataField name="Temperature (K)" fld="1" baseField="0" baseItem="0"/>
   </dataFields>
   <chartFormats count="1">
     <chartFormat chart="0" format="0" series="1">
@@ -6876,9 +7009,9 @@
     <pivotHierarchy dragToData="1"/>
     <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
     <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
+    <pivotHierarchy dragToData="1" caption="Temperature (K)"/>
     <pivotHierarchy dragToData="1"/>
     <pivotHierarchy dragToData="1"/>
-    <pivotHierarchy dragToData="1" caption="Density (kg/m^3)"/>
     <pivotHierarchy dragToData="1"/>
   </pivotHierarchies>
   <rowHierarchiesUsage count="1">
@@ -6889,320 +7022,310 @@
       <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" calculatedMembersInFilters="1" hideValuesRow="1"/>
     </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{44433962-1CF7-4059-B4EE-95C3D5FFCF73}">
-      <x15:pivotTableData rowCount="63" columnCount="1" cacheId="806323974">
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>42.292560000000002</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>38.37903</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>34.748750000000001</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>31.38721</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>28.28031</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>25.41433</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>22.776029999999999</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>20.35257</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>18.13148</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>16.10078</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>14.24883</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>12.564120000000001</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>10.73124</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>9.1657510000000002</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>7.828633</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>6.6865769999999998</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>5.7111270000000003</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>4.8779779999999997</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>4.1663680000000003</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>3.5585710000000002</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>3.039364</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>2.5849820000000001</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>2.2001719999999998</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>1.8740159999999999</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>1.5973740000000001</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>1.3625579999999999</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>1.163089</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>0.99352839999999998</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>0.84928090000000001</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>0.72648230000000003</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>0.62187110000000001</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>0.53268590000000005</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>0.45658749999999998</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>0.3888161</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>0.33174389999999998</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>0.28358420000000001</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>0.24286250000000001</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>0.20836250000000001</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>0.1790783</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>0.15417439999999999</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>0.13295689999999999</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>0.1148479</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>9.9364759999999996E-2</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>8.6104189999999997E-2</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>7.4728000000000003E-2</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>6.4952609999999994E-2</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>5.6539279999999997E-2</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>4.9284790000000002E-2</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>4.344046E-2</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>3.8289160000000003E-2</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>3.3748720000000003E-2</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>2.9746539999999998E-2</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>2.6475800000000001E-2</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>2.3535819999999999E-2</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>2.0896209999999998E-2</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>1.8528929999999999E-2</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>1.640844E-2</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>1.451125E-2</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>1.281594E-2</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>1.1302939999999999E-2</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>9.9543470000000005E-3</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>8.7538979999999995E-3</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>378.18004488500003</x15:v>
+      <x15:pivotTableData rowCount="61" columnCount="1" cacheId="133619859">
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>288.14999999999998</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>281.64999999999998</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>275.14999999999998</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>268.64999999999998</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>262.14999999999998</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>255.65</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>249.15</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>242.65</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>236.15</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>229.65</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>223.15</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>216.65</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>216.65</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>216.65</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>216.65</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>216.65</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>216.65</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>216.65</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>216.65</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>216.65</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>216.65</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>217.65</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>218.65</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>219.65</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>220.65</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>221.65</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>222.65</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>223.65</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>224.65</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>225.65</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>226.65</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>227.65</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>228.65</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>231.45</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>234.25</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>237.05</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>239.85</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>242.65</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>245.45</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>248.25</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>251.05</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>253.85</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>256.64999999999998</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>259.45</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>262.25</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>265.05</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>267.85000000000002</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>270.64999999999998</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>270.64999999999998</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>270.64999999999998</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>270.64999999999998</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>270.64999999999998</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>267.85000000000002</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>265.05</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>262.25</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>259.45</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>256.64999999999998</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>253.85</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>251.05</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>248.25</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>14569.2</x15:v>
           </x15:c>
         </x15:pivotRow>
       </x15:pivotTableData>
@@ -7220,11 +7343,11 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D8A81E05-F159-40FB-B4C0-5B4D59235038}" name="PivotChartTable2" cacheId="54" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
-  <location ref="A1:B64" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D8A81E05-F159-40FB-B4C0-5B4D59235038}" name="PivotChartTable2" cacheId="8" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+  <location ref="A1:B62" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="2">
     <pivotField axis="axisRow" allDrilled="1" subtotalTop="0" showAll="0" dataSourceSort="1" defaultSubtotal="0" defaultAttributeDrillState="1">
-      <items count="62">
+      <items count="60">
         <item x="0"/>
         <item x="1"/>
         <item x="2"/>
@@ -7285,8 +7408,6 @@
         <item x="57"/>
         <item x="58"/>
         <item x="59"/>
-        <item x="60"/>
-        <item x="61"/>
       </items>
     </pivotField>
     <pivotField dataField="1" subtotalTop="0" showAll="0" defaultSubtotal="0"/>
@@ -7294,7 +7415,7 @@
   <rowFields count="1">
     <field x="0"/>
   </rowFields>
-  <rowItems count="63">
+  <rowItems count="61">
     <i>
       <x/>
     </i>
@@ -7474,12 +7595,6 @@
     </i>
     <i>
       <x v="59"/>
-    </i>
-    <i>
-      <x v="60"/>
-    </i>
-    <i>
-      <x v="61"/>
     </i>
     <i t="grand">
       <x/>
@@ -7522,7 +7637,7 @@
       <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" calculatedMembersInFilters="1" hideValuesRow="1"/>
     </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{44433962-1CF7-4059-B4EE-95C3D5FFCF73}">
-      <x15:pivotTableData rowCount="63" columnCount="1" cacheId="502512662">
+      <x15:pivotTableData rowCount="61" columnCount="1" cacheId="502512662">
         <x15:pivotRow count="1">
           <x15:c>
             <x15:v>101325</x15:v>
@@ -7825,17 +7940,7 @@
         </x15:pivotRow>
         <x15:pivotRow count="1">
           <x15:c>
-            <x15:v>20.31467</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>17.661020000000001</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>793792.16428000014</x15:v>
+            <x15:v>793754.18859000015</x15:v>
           </x15:c>
         </x15:pivotRow>
       </x15:pivotTableData>
@@ -7853,11 +7958,11 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{DB5B6DDB-B8C0-414A-9782-056CB44D8C3F}" name="PivotChartTable1" cacheId="45" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
-  <location ref="A1:B64" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E6EBDEBF-0633-40E3-AAE5-FBE9E430F117}" name="PivotChartTable3" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+  <location ref="A1:B62" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="2">
     <pivotField axis="axisRow" allDrilled="1" subtotalTop="0" showAll="0" dataSourceSort="1" defaultSubtotal="0" defaultAttributeDrillState="1">
-      <items count="62">
+      <items count="60">
         <item x="0"/>
         <item x="1"/>
         <item x="2"/>
@@ -7918,8 +8023,6 @@
         <item x="57"/>
         <item x="58"/>
         <item x="59"/>
-        <item x="60"/>
-        <item x="61"/>
       </items>
     </pivotField>
     <pivotField dataField="1" subtotalTop="0" showAll="0" defaultSubtotal="0"/>
@@ -7927,7 +8030,7 @@
   <rowFields count="1">
     <field x="0"/>
   </rowFields>
-  <rowItems count="63">
+  <rowItems count="61">
     <i>
       <x/>
     </i>
@@ -8107,12 +8210,6 @@
     </i>
     <i>
       <x v="59"/>
-    </i>
-    <i>
-      <x v="60"/>
-    </i>
-    <i>
-      <x v="61"/>
     </i>
     <i t="grand">
       <x/>
@@ -8122,7 +8219,7 @@
     <i/>
   </colItems>
   <dataFields count="1">
-    <dataField name="Temperature (K)" fld="1" baseField="0" baseItem="0"/>
+    <dataField name="Density (kg/m^3)" fld="1" baseField="0" baseItem="8"/>
   </dataFields>
   <chartFormats count="1">
     <chartFormat chart="0" format="0" series="1">
@@ -8142,9 +8239,9 @@
     <pivotHierarchy dragToData="1"/>
     <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
     <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
-    <pivotHierarchy dragToData="1" caption="Temperature (K)"/>
     <pivotHierarchy dragToData="1"/>
     <pivotHierarchy dragToData="1"/>
+    <pivotHierarchy dragToData="1" caption="Density (kg/m^3)"/>
     <pivotHierarchy dragToData="1"/>
   </pivotHierarchies>
   <rowHierarchiesUsage count="1">
@@ -8155,320 +8252,310 @@
       <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" calculatedMembersInFilters="1" hideValuesRow="1"/>
     </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{44433962-1CF7-4059-B4EE-95C3D5FFCF73}">
-      <x15:pivotTableData rowCount="63" columnCount="1" cacheId="133619859">
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>288.14999999999998</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>281.64999999999998</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>275.14999999999998</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>268.64999999999998</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>262.14999999999998</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>255.65</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>249.15</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>242.65</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>236.15</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>229.65</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>223.15</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>216.65</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>216.65</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>216.65</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>216.65</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>216.65</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>216.65</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>216.65</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>216.65</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>216.65</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>216.65</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>217.65</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>218.65</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>219.65</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>220.65</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>221.65</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>222.65</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>223.65</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>224.65</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>225.65</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>226.65</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>227.65</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>228.65</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>231.45</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>234.25</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>237.05</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>239.85</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>242.65</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>245.45</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>248.25</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>251.05</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>253.85</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>256.64999999999998</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>259.45</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>262.25</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>265.05</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>267.85000000000002</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>270.64999999999998</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>270.64999999999998</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>270.64999999999998</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>270.64999999999998</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>270.64999999999998</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>267.85000000000002</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>265.05</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>262.25</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>259.45</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>256.64999999999998</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>253.85</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>251.05</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>248.25</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>245.45</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>242.65</x15:v>
-          </x15:c>
-        </x15:pivotRow>
-        <x15:pivotRow count="1">
-          <x15:c>
-            <x15:v>15057.299999999994</x15:v>
+      <x15:pivotTableData rowCount="61" columnCount="1" cacheId="806323974">
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>1.224979</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>1.111626</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>1.0064770000000001</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>0.90911189999999997</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>0.81912209999999996</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>0.73611070000000001</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>0.65969409999999995</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>0.58949980000000002</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>0.52516750000000001</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>0.46634940000000003</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>0.41270869999999998</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>0.36391230000000002</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>0.31082399999999999</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>0.26548050000000001</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>0.2267517</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>0.1936727</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>0.16541939999999999</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>0.14128769999999999</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>0.1206764</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>0.10307189999999999</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>8.8033349999999996E-2</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>7.4872469999999997E-2</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>6.3726660000000004E-2</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>5.4279750000000002E-2</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>4.6266969999999998E-2</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>3.9465680000000003E-2</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>3.3688170000000003E-2</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>2.8776949999999999E-2</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>2.4598910000000002E-2</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>2.1042129999999999E-2</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>1.801212E-2</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>1.542893E-2</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>1.322478E-2</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>1.1261820000000001E-2</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>9.6087610000000004E-3</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>8.2138449999999991E-3</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>7.0343660000000002E-3</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>6.0350960000000002E-3</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>5.1868940000000001E-3</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>4.4655679999999996E-3</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>3.8510179999999999E-3</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>3.3265E-3</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>2.878041E-3</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>2.4939559999999999E-3</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>2.1644519999999999E-3</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>1.8813129999999999E-3</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>1.6376260000000001E-3</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>1.4275049999999999E-3</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>1.258227E-3</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>1.109023E-3</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>9.7751159999999991E-4</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>8.6159080000000002E-4</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>7.6685580000000004E-4</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>6.8170079999999998E-4</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>6.0524609999999996E-4</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>5.3667929999999997E-4</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>4.7526069999999999E-4</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>4.2030950000000001E-4</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>3.7120600000000001E-4</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>0</x15:v>
+          </x15:c>
+        </x15:pivotRow>
+        <x15:pivotRow count="1">
+          <x15:c>
+            <x15:v>10.952890041600002</x15:v>
           </x15:c>
         </x15:pivotRow>
       </x15:pivotTableData>
@@ -8785,7 +8872,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R29" sqref="R29"/>
+      <selection activeCell="J33" sqref="J33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>